<commit_message>
Deploying to gh-pages from  @ 002505b587daa6059671603c0ad7f97573af2964 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.5.2.xlsx
+++ b/en/downloads/data-excel/1.5.2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="52">
   <si>
     <t>Көрсөткүчтөрдүн аталышы</t>
   </si>
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +963,9 @@
         <f>P7/P8*100</f>
         <v>5.2301500219592005E-2</v>
       </c>
-      <c r="Q6" s="32"/>
+      <c r="Q6" s="32">
+        <v>4.4166007693658721E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -1067,7 +1069,9 @@
       <c r="P8" s="34">
         <v>619102.69999999995</v>
       </c>
-      <c r="Q8" s="34"/>
+      <c r="Q8" s="34">
+        <v>601820.30000000005</v>
+      </c>
     </row>
     <row r="9" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
@@ -1156,7 +1160,9 @@
         <f>P11/P12*100</f>
         <v>0.11389691583067656</v>
       </c>
-      <c r="Q10" s="32"/>
+      <c r="Q10" s="32">
+        <v>0.36185407133694547</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1260,7 +1266,9 @@
       <c r="P12" s="34">
         <v>20105.900000000001</v>
       </c>
-      <c r="Q12" s="34"/>
+      <c r="Q12" s="34">
+        <v>20892.400000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
@@ -1349,7 +1357,9 @@
         <f>P15/P16*100</f>
         <v>0.23462986721450702</v>
       </c>
-      <c r="Q14" s="32"/>
+      <c r="Q14" s="32">
+        <v>0.27408710679222598</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1453,7 +1463,9 @@
       <c r="P16" s="38">
         <v>71943.100000000006</v>
       </c>
-      <c r="Q16" s="38"/>
+      <c r="Q16" s="38">
+        <v>63884.800000000003</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
@@ -1542,7 +1554,9 @@
         <f>P19/P20*100</f>
         <v>1.3155087819099765E-2</v>
       </c>
-      <c r="Q18" s="32"/>
+      <c r="Q18" s="32">
+        <v>4.6658384803364067E-4</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
@@ -1646,7 +1660,9 @@
       <c r="P20" s="38">
         <v>84378</v>
       </c>
-      <c r="Q20" s="38"/>
+      <c r="Q20" s="38">
+        <v>85729.5</v>
+      </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
@@ -1734,7 +1750,9 @@
       <c r="P22" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="Q22" s="32"/>
+      <c r="Q22" s="32">
+        <v>8.6032657053793982E-2</v>
+      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
@@ -1838,7 +1856,9 @@
       <c r="P24" s="38">
         <v>14806.7</v>
       </c>
-      <c r="Q24" s="38"/>
+      <c r="Q24" s="38">
+        <v>16970.3</v>
+      </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
@@ -1927,7 +1947,9 @@
         <f>P27/P28*100</f>
         <v>5.8984602750043668E-3</v>
       </c>
-      <c r="Q26" s="32"/>
+      <c r="Q26" s="32" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
@@ -2031,7 +2053,9 @@
       <c r="P28" s="38">
         <v>44079.3</v>
       </c>
-      <c r="Q28" s="38"/>
+      <c r="Q28" s="38">
+        <v>47183.5</v>
+      </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
@@ -2119,7 +2143,9 @@
       <c r="P30" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="Q30" s="32"/>
+      <c r="Q30" s="32" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
@@ -2223,7 +2249,9 @@
       <c r="P32" s="38">
         <v>16531.2</v>
       </c>
-      <c r="Q32" s="38"/>
+      <c r="Q32" s="38">
+        <v>17405.3</v>
+      </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
@@ -2310,7 +2338,9 @@
         <f>P35/P36*100</f>
         <v>2.3302011546146723E-3</v>
       </c>
-      <c r="Q34" s="32"/>
+      <c r="Q34" s="32">
+        <v>1.1900270969169968E-5</v>
+      </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
@@ -2414,7 +2444,9 @@
       <c r="P36" s="38">
         <v>85829.5</v>
       </c>
-      <c r="Q36" s="38"/>
+      <c r="Q36" s="38">
+        <v>84031.7</v>
+      </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
@@ -2498,7 +2530,9 @@
         <f>P39/P40*100</f>
         <v>4.6929382203002752E-2</v>
       </c>
-      <c r="Q38" s="32"/>
+      <c r="Q38" s="32" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
@@ -2602,7 +2636,9 @@
       <c r="P40" s="35">
         <v>247179.9</v>
       </c>
-      <c r="Q40" s="35"/>
+      <c r="Q40" s="35">
+        <v>231841.7</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
@@ -2686,7 +2722,9 @@
         <f>P43/P44*100</f>
         <v>1.16791390138719E-3</v>
       </c>
-      <c r="Q42" s="32"/>
+      <c r="Q42" s="32" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
@@ -2790,7 +2828,9 @@
       <c r="P44" s="40">
         <v>34249.1</v>
       </c>
-      <c r="Q44" s="40"/>
+      <c r="Q44" s="40">
+        <v>33881.1</v>
+      </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 9b0ac4fb70da3d384ca3b7cc3a5d52cc67b9c9ee 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.5.2.xlsx
+++ b/en/downloads/data-excel/1.5.2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="52">
   <si>
     <t>Көрсөткүчтөрдүн аталышы</t>
   </si>
@@ -764,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q66"/>
+  <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +778,7 @@
     <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -789,7 +789,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
@@ -809,7 +809,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -823,7 +823,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -875,8 +875,11 @@
       <c r="Q4" s="14">
         <v>2020</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="14">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -900,8 +903,9 @@
       <c r="O5" s="34"/>
       <c r="P5" s="34"/>
       <c r="Q5" s="34"/>
-    </row>
-    <row r="6" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R5" s="34"/>
+    </row>
+    <row r="6" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>41</v>
       </c>
@@ -966,8 +970,12 @@
       <c r="Q6" s="32">
         <v>4.4166007693658721E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="32">
+        <f>R7/R8*100</f>
+        <v>0.26112215360929741</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>44</v>
       </c>
@@ -1019,8 +1027,11 @@
       <c r="Q7" s="34">
         <v>265.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="34">
+        <v>1931.83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>42</v>
       </c>
@@ -1072,8 +1083,11 @@
       <c r="Q8" s="34">
         <v>601820.30000000005</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R8" s="34">
+        <v>739818.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>6</v>
       </c>
@@ -1097,8 +1111,9 @@
       <c r="O9" s="32"/>
       <c r="P9" s="32"/>
       <c r="Q9" s="32"/>
-    </row>
-    <row r="10" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R9" s="32"/>
+    </row>
+    <row r="10" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>41</v>
       </c>
@@ -1163,8 +1178,12 @@
       <c r="Q10" s="32">
         <v>0.36185407133694547</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" s="32">
+        <f>R11/R12*100</f>
+        <v>6.1995480785353285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>44</v>
       </c>
@@ -1216,8 +1235,11 @@
       <c r="Q11" s="34">
         <v>75.599999999999994</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" s="34">
+        <v>1552.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>42</v>
       </c>
@@ -1269,8 +1291,11 @@
       <c r="Q12" s="34">
         <v>20892.400000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R12" s="34">
+        <v>25048.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>9</v>
       </c>
@@ -1294,8 +1319,9 @@
       <c r="O13" s="39"/>
       <c r="P13" s="39"/>
       <c r="Q13" s="39"/>
-    </row>
-    <row r="14" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R13" s="39"/>
+    </row>
+    <row r="14" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>41</v>
       </c>
@@ -1360,8 +1386,12 @@
       <c r="Q14" s="32">
         <v>0.27408710679222598</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="32">
+        <f>R15/R16*100</f>
+        <v>0.15289385371573422</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
@@ -1413,8 +1443,11 @@
       <c r="Q15" s="34">
         <v>175.1</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15" s="34">
+        <v>125.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>42</v>
       </c>
@@ -1466,8 +1499,11 @@
       <c r="Q16" s="38">
         <v>63884.800000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="38">
+        <v>82213.899999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>12</v>
       </c>
@@ -1491,8 +1527,9 @@
       <c r="O17" s="34"/>
       <c r="P17" s="34"/>
       <c r="Q17" s="34"/>
-    </row>
-    <row r="18" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R17" s="34"/>
+    </row>
+    <row r="18" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>41</v>
       </c>
@@ -1557,8 +1594,12 @@
       <c r="Q18" s="32">
         <v>4.6658384803364067E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="32">
+        <f>R19/R20*100</f>
+        <v>0.12440731654917085</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>44</v>
       </c>
@@ -1610,8 +1651,11 @@
       <c r="Q19" s="34">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="34">
+        <v>99.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>42</v>
       </c>
@@ -1663,8 +1707,11 @@
       <c r="Q20" s="38">
         <v>85729.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20" s="38">
+        <v>80059.600000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>15</v>
       </c>
@@ -1688,8 +1735,9 @@
       <c r="O21" s="34"/>
       <c r="P21" s="34"/>
       <c r="Q21" s="34"/>
-    </row>
-    <row r="22" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R21" s="34"/>
+    </row>
+    <row r="22" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>41</v>
       </c>
@@ -1753,8 +1801,12 @@
       <c r="Q22" s="32">
         <v>8.6032657053793982E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="32">
+        <f>R23/R24*100</f>
+        <v>5.2408765074798951E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>44</v>
       </c>
@@ -1806,8 +1858,11 @@
       <c r="Q23" s="34">
         <v>14.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" s="34">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>42</v>
       </c>
@@ -1859,8 +1914,11 @@
       <c r="Q24" s="38">
         <v>16970.3</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24" s="38">
+        <v>17172.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>18</v>
       </c>
@@ -1884,8 +1942,9 @@
       <c r="O25" s="34"/>
       <c r="P25" s="34"/>
       <c r="Q25" s="34"/>
-    </row>
-    <row r="26" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R25" s="34"/>
+    </row>
+    <row r="26" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>41</v>
       </c>
@@ -1950,8 +2009,12 @@
       <c r="Q26" s="32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26" s="32">
+        <f>R27/R28*100</f>
+        <v>2.8058906055606046E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>44</v>
       </c>
@@ -2003,8 +2066,11 @@
       <c r="Q27" s="34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" s="34">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>42</v>
       </c>
@@ -2056,8 +2122,11 @@
       <c r="Q28" s="38">
         <v>47183.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28" s="38">
+        <v>56666.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>21</v>
       </c>
@@ -2081,8 +2150,9 @@
       <c r="O29" s="34"/>
       <c r="P29" s="34"/>
       <c r="Q29" s="34"/>
-    </row>
-    <row r="30" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R29" s="34"/>
+    </row>
+    <row r="30" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>41</v>
       </c>
@@ -2146,8 +2216,12 @@
       <c r="Q30" s="32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30" s="32">
+        <f>R31/R32*100</f>
+        <v>0.19015052770834487</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>44</v>
       </c>
@@ -2199,8 +2273,11 @@
       <c r="Q31" s="34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31" s="34">
+        <v>58.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>42</v>
       </c>
@@ -2252,8 +2329,11 @@
       <c r="Q32" s="38">
         <v>17405.3</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32" s="38">
+        <v>30765.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
         <v>24</v>
       </c>
@@ -2277,8 +2357,9 @@
       <c r="O33" s="34"/>
       <c r="P33" s="34"/>
       <c r="Q33" s="34"/>
-    </row>
-    <row r="34" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R33" s="34"/>
+    </row>
+    <row r="34" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>41</v>
       </c>
@@ -2341,8 +2422,12 @@
       <c r="Q34" s="32">
         <v>1.1900270969169968E-5</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34" s="32">
+        <f>R35/R36*100</f>
+        <v>7.1009394461267222E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>44</v>
       </c>
@@ -2394,8 +2479,11 @@
       <c r="Q35" s="34">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35" s="34">
+        <v>78.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>42</v>
       </c>
@@ -2447,8 +2535,11 @@
       <c r="Q36" s="38">
         <v>84031.7</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36" s="38">
+        <v>110267.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>27</v>
       </c>
@@ -2472,8 +2563,9 @@
       <c r="O37" s="34"/>
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
-    </row>
-    <row r="38" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R37" s="34"/>
+    </row>
+    <row r="38" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>41</v>
       </c>
@@ -2533,8 +2625,11 @@
       <c r="Q38" s="32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>44</v>
       </c>
@@ -2586,8 +2681,11 @@
       <c r="Q39" s="34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>42</v>
       </c>
@@ -2639,8 +2737,11 @@
       <c r="Q40" s="35">
         <v>231841.7</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R40" s="35">
+        <v>297797.59999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>30</v>
       </c>
@@ -2664,8 +2765,9 @@
       <c r="O41" s="34"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="34"/>
-    </row>
-    <row r="42" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R41" s="34"/>
+    </row>
+    <row r="42" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>41</v>
       </c>
@@ -2725,8 +2827,11 @@
       <c r="Q42" s="32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R42" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>44</v>
       </c>
@@ -2778,8 +2883,11 @@
       <c r="Q43" s="34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R43" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="26" t="s">
         <v>42</v>
       </c>
@@ -2831,8 +2939,11 @@
       <c r="Q44" s="40">
         <v>33881.1</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44" s="40">
+        <v>39827.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>46</v>
       </c>
@@ -2855,7 +2966,7 @@
       <c r="N45" s="16"/>
       <c r="O45" s="16"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2869,7 +2980,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2883,7 +2994,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>

</xml_diff>